<commit_message>
Cap nhat MMO 230514
</commit_message>
<xml_diff>
--- a/MMO/MMO-230512.xlsx
+++ b/MMO/MMO-230512.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Clone Desiccant\Desiccant\MMO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A99A078-418D-4DA9-9F95-ABC525BEA84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760" tabRatio="618" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="618" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Camtu082880" sheetId="1" r:id="rId1"/>
@@ -15,12 +21,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Link!$A$5:$E$60</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="411">
   <si>
     <t>Stt</t>
   </si>
@@ -911,63 +918,7 @@
   </si>
   <si>
     <r>
-      <t>#cryptoshi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> (update v2)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>#scoinclick</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> (update v3)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>#claimfreebitsxyz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> (update v2)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>#888satoshis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> (update v2)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>#oldwor</t>
     </r>
     <r>
       <rPr>
@@ -1009,20 +960,6 @@
   </si>
   <si>
     <r>
-      <t>#dutchycorp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> (offline)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>#firefaucet</t>
     </r>
     <r>
@@ -1235,12 +1172,282 @@
   <si>
     <t>https://www.mediafire.com/file/3gy6dwzptnlb6zv/HarshcoinV2.zip</t>
   </si>
+  <si>
+    <t>https://buxcoin.io/?r=145676</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/3c9zzks55pt2c8l/Buxcoin.zip/file</t>
+  </si>
+  <si>
+    <t>https://freecoinz.net/?r=6303</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/cdgue7cmjtm6aah/Freecoinz.zip/file</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/k8qjles32tajnnh/Cryptonline.zip/file</t>
+  </si>
+  <si>
+    <t>https://bestcripto.xyz/?r=60446</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/p9vruf4jceng0p7/Bestcripto.zip/file</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/vaq1bttb6dcki1c/Freeshiba.zip/file</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/iyigvnri2kn1ykc/Multicoins.zip/file</t>
+  </si>
+  <si>
+    <t>https://ptc4btc.com/?r=58802</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/ras71n0qkbd59ie/Ptc4btc.zip/file</t>
+  </si>
+  <si>
+    <t>https://coinoto.net/?r=91809</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/c0944sffxmkfkon/Coinoto.zip/file</t>
+  </si>
+  <si>
+    <t>https://bitcointricks.com/?ref=30266</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/0wzf9cop3n78s7w/Bitcointricks.zip/file</t>
+  </si>
+  <si>
+    <t>https://cryptofenz.xyz/?r=18YBEFuQ27Xo7544SET7zFEoBjFRyX1WgV</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/mf8r8cy3oqcw6tk/Cryptofenz.zip/file</t>
+  </si>
+  <si>
+    <t>https://tokenmix.pro/?r=C_pFRzYHql</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/f3xce5v13gyvqho/Tokenmix.zip/file</t>
+  </si>
+  <si>
+    <t>https://paybits.xyz/?r=FiJlA5Mwvh</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/qiohajw9k3uh1xz/Paybits.zip/file</t>
+  </si>
+  <si>
+    <t>https://topfaucet.click/?r=AqcrHUb4ZB5</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/wnnihnlhtf6gh2b/TopfaucetV3.zip/file</t>
+  </si>
+  <si>
+    <t>https://autofaucet.org/r/Vuongphong</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/7lchbnsjfuu15fi/Autofaucet.zip/file</t>
+  </si>
+  <si>
+    <t>https://autoclaim.in/r/Vuongphong</t>
+  </si>
+  <si>
+    <t>https://autobitco.in/r/Vuongphong</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/vnq5rzod405t9jp/Autoclaim.zip/file</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/2cz2su7m5liu9qp/Autobitco.zip/file</t>
+  </si>
+  <si>
+    <t>https://btcad24.com/?r=890</t>
+  </si>
+  <si>
+    <t>https://upfiles.download/file/download/eyJpdiI6IjBNSkZNQlh2eHdxeEE3NURCUTFsL0E9PSIsInZhbHVlIjoiVEhMNnJsdHM4OGx5alo4VjhQMXY5b0lYTElGTFlWQWZqTnBDNWM4OUsyMmFreUFlRkxiWE1USkkxVGxCaE5MWmZZRzNzc2F1dGd5ckF6YkpaVmN6eFhPKytOSGlkaDZOMTNQSUxHSnIzOFlRTEd3Ky9nSHVFczJ4alQxNTRnc0NkaGtuZm94NVdKRURGRmx0eGFzM0FSVVY5ajU4eFExWFpmNU02QUZmUEtwUkEyTThxYmhPN1V0QlMvQ0E4d081eXBBckpkS2t5Zkt5eW16cEphVERuU0JlYXpRQ0FRTWtJZGtFazlGa3BwYU1nZzdHMFg2dGt3TjZpbUlGSGlqNzZyV3JIZ2YrRm1mYVoxWWJCSkpVbkE9PSIsIm1hYyI6ImFmNjY2YjlkNGNjZmEyMDIyMzE3MTBjYTY0OGFkZjY3ZTg3ZjU4YTk0ZGU3ZDFkZWMyNjZmNTAwZjg2MmE0MTkiLCJ0YWciOiIifQ==?expires=1684019630&amp;signature=dd38470d5a0f61204d6936bad9a21870632069ac0ed2b1fe5286bc3d336ea40e</t>
+  </si>
+  <si>
+    <t>#cryptoshi (update v2)</t>
+  </si>
+  <si>
+    <t>https://ziifaucet.com/?r=4741</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/i4uqrc91ltd733r/Ziifaucet.zip/file</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/38o7qh44jzbvcir/Snails.zip/file</t>
+  </si>
+  <si>
+    <t>#scoinclick (update v3)</t>
+  </si>
+  <si>
+    <t>#claimfreebitsxyz (update v2)</t>
+  </si>
+  <si>
+    <t>https://cryptoclaim.club?r=5175</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/domv9wo3a2svijo/Cryptoclaim.zip/file</t>
+  </si>
+  <si>
+    <t>https://lemeclaim.xyz?r=10590</t>
+  </si>
+  <si>
+    <t>10 tiếng</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/kapk3ffy0ksa4zg/Lemeclaim.zip/file</t>
+  </si>
+  <si>
+    <t>https://cryptofy.club?r=10102</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/tsaaf4ny3oqdmif/Cryptofy.zip/file</t>
+  </si>
+  <si>
+    <t>https://bestautofaucet.com/?r=1TDjHJfyo</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/q209iwgc1tfznea/Bestautofaucet.zip/file</t>
+  </si>
+  <si>
+    <t>https://sevenfaucet.com/ref/4078</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/yj8rrcqtzde2aho/Sevenfaucet.zip/file</t>
+  </si>
+  <si>
+    <t>https://landofbits.com/?r=3987</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/bgyej3vw9wljv7v/Landofbits.zip/file</t>
+  </si>
+  <si>
+    <t>https://888satoshis.com/?r=55396</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/6yft22li4e9b13o/888satoshisV2.zip/file</t>
+  </si>
+  <si>
+    <t>https://faucet.pk/?r=5957</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/tu5dgc4qq4dttyz/Faucetpk.zip/file</t>
+  </si>
+  <si>
+    <t>https://welovebtc.net/?r=10485</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/lopsl8wkmg4blai/Welovebtc.zip/file</t>
+  </si>
+  <si>
+    <t>#oldwor (update v2)</t>
+  </si>
+  <si>
+    <t>https://faucetofbob.xyz/?ref=70648</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/l2c348kh3qmt9h4/Faucetofbob.zip/file</t>
+  </si>
+  <si>
+    <t>https://faucetcrypto.eu/?r=3576</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/omwdrn6wuyfw0r9/Faucetcryptoeu.zip/file</t>
+  </si>
+  <si>
+    <t>https://uptocoin.my.id/?r=1887</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/fufyw71ftsfx71d/Uptocoin.zip/file</t>
+  </si>
+  <si>
+    <t>https://aruble.net/?r=oRxL6RSevc</t>
+  </si>
+  <si>
+    <t>https://mycryptofaucet.eu/?ref=5605</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/as0n7297f8tfw9s/Mycryptofaucet.zip/file</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/83wsv94p17hz0xg/GwaherV4.zip/file</t>
+  </si>
+  <si>
+    <t>https://tronminingfarm.com/?ref=Vuongphong</t>
+  </si>
+  <si>
+    <t>https://gwaher.com/</t>
+  </si>
+  <si>
+    <t>https://luckydice.net/?r=18YBEFuQ27Xo7544SET7zFEoBjFRyX1WgV</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/jehv2jjrw63fjz1/LuckydiceV5.zip/file</t>
+  </si>
+  <si>
+    <t>https://flashearn.pw/?r=159428</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/hohnr0nk163m6n0/Flashearn.zip/file</t>
+  </si>
+  <si>
+    <t>https://claimfreecoins.io/tron-faucet/?r=TPTy5jGEeATLSCkWkJAaDbx8aqeYqGzhbz</t>
+  </si>
+  <si>
+    <t>#dutchycorp (offline)</t>
+  </si>
+  <si>
+    <t>https://firefaucet.win/ref/Vuongphong</t>
+  </si>
+  <si>
+    <t>https://upfiles.download/file/download/eyJpdiI6IlRQZUtLN1EzRkR6UExSYkx4d3lZWEE9PSIsInZhbHVlIjoia3Y2S21hUHJGK2RqWkE4R2lwTzM2cW16RnNtUzl4eVRBZWQxYjcrVE9uY3UrdVhxWWlVaFpSenNPUDN1b3V5NUc5dlJqQ2FHbDdPVXVzWU1QVjdyTDhRSlpoK2s0NThPQkhBdldtclJKajVMdjM1UTlFMTFHK3pwdHZZTWsyZDZ4S3BjU1VKWEZzVVFzd1ZxeUFaL2I3TnBzZmRjRklRK3RPUEdCMjFtUDF3c3AxeGtSQzYxeTdHRzM2UG9OK1Qxd0ttSnhnd0hkVTF5V3JnNVo1TXEzcUFCMlFKTmFmQ21FUDhSL1liUVRCbGxPamMrS2xNOVV2ZnBRcjVKMi9pTjBNRVB5TkluZnVjZWpydndXdVl5K1E9PSIsIm1hYyI6IjhkOWUxN2M0ZmMxNzk0ODM4MTNjMjNkNzM3M2U1MTUxNzI0MDBhZDY1MjBiYjc5NTk4NjUyMDQ3YTNhYTQ1ZmEiLCJ0YWciOiIifQ==?expires=1684042652&amp;signature=0146e880dc3f8d169a7e14150d12a5b9b279de7a37421c03c6f4e5c36c852102</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/l087oy2rkchrnsg/Coinbirds.zip/file</t>
+  </si>
+  <si>
+    <t>https://cashmining.me/?ref=24679</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/icsj2achalx71zj/Cashmining.zip/file</t>
+  </si>
+  <si>
+    <t>https://payfee.xyz/?r=TPTy5jGEeATLSCkWkJAaDbx8aqeYqGzhbz</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/ems020n0glivp32/Payfee.zip/file</t>
+  </si>
+  <si>
+    <t>https://cekip.site/ref/5684</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/fuklwjmsve9ncam/CekipV2.zip/file</t>
+  </si>
+  <si>
+    <t>https://icucu.icu/doge/ref/mdrnkddsjpjr</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/2hcp2nye8rjc7ow/Icucu.zip/file</t>
+  </si>
+  <si>
+    <t>https://battle-farm.com/?aff=235472</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/rgmvqg4u54zt15x/Battlefarm.zip/file</t>
+  </si>
+  <si>
+    <t>http://btccolletor.xyz/?r=3639</t>
+  </si>
+  <si>
+    <t>https://www.mediafire.com/file/in45cbbkelild1x/Btccolletor.zip/file</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1295,6 +1502,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1329,7 +1542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1346,18 +1559,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1366,6 +1572,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1376,6 +1583,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1636,14 +1846,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:M35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -1712,322 +1922,317 @@
       </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
       <c r="H6" s="9"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="10" t="s">
+      <c r="I7" t="s">
         <v>145</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7">
         <v>5948331720</v>
       </c>
-      <c r="M7" s="10" t="str">
+      <c r="M7" t="str">
         <f>CONCATENATE("default|",B7,":",C7,":",D7,"|http|",G7,"|",J7,"|",K7,"|",L7,"|")</f>
         <v>default|camtu082880@gmail.com:minhtu:*minhanh#|http|42.118.228.99||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10" t="str">
+      <c r="C8" t="str">
         <f>MID(B8,1,LEN(B8)-10)</f>
         <v>camtu082880</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8">
         <v>5948331720</v>
       </c>
-      <c r="M8" s="10" t="str">
+      <c r="M8" t="str">
         <f t="shared" ref="M8:M14" si="0">CONCATENATE("default|",B8,":",C8,":",D8,"|http|",G8,"|",J8,"|",K8,"|",L8,"|")</f>
         <v>default|camtu082880@gmail.com:camtu082880:*minhanh#|http|42.118.228.99||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+    <row r="9" spans="1:13" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>3</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="10">
         <v>5948331720</v>
       </c>
-      <c r="M9" s="13" t="str">
+      <c r="M9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>default|camtu082880@gmail.com::*minhanh#|http|42.118.228.99||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" t="s">
         <v>146</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10">
         <v>5948331720</v>
       </c>
-      <c r="M10" s="10" t="str">
+      <c r="M10" t="str">
         <f t="shared" si="0"/>
         <v>default|camtu082880@gmail.com::minhanh|http|42.118.228.99||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
+    <row r="11" spans="1:13" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="10">
         <v>5948331720</v>
       </c>
-      <c r="M11" s="13" t="str">
+      <c r="M11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>default|camtu082880@gmail.com:minhtu:*minhanh#|http|42.118.228.99||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="10">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="10" t="str">
+      <c r="C12" t="str">
         <f>MID(B12,1,LEN(B12)-10)</f>
         <v>camtu082880</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="10" t="s">
+      <c r="I12" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K12" t="s">
         <v>10</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12">
         <v>5948331720</v>
       </c>
-      <c r="M12" s="10" t="str">
+      <c r="M12" t="str">
         <f t="shared" si="0"/>
         <v>default|camtu082880@gmail.com:camtu082880:*minhanh#|http|183.80.65.178||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>7</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="10" t="str">
+      <c r="C13" t="str">
         <f>MID(B13,1,LEN(B13)-10)</f>
         <v>camtu082880</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="10" t="s">
+      <c r="I13" t="s">
         <v>147</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13">
         <v>5948331720</v>
       </c>
-      <c r="M13" s="10" t="str">
+      <c r="M13" t="str">
         <f t="shared" si="0"/>
         <v>default|camtu082880@gmail.com:camtu082880:*minhanh#|http|183.80.65.178||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13">
+    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <v>8</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="13" t="str">
+      <c r="C14" s="10" t="str">
         <f>MID(B14,1,LEN(B14)-10)</f>
         <v>camtu082880</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="13" t="s">
+      <c r="H14" s="12"/>
+      <c r="I14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="10">
         <v>5948331720</v>
       </c>
-      <c r="M14" s="13" t="str">
+      <c r="M14" s="10" t="str">
         <f t="shared" si="0"/>
         <v>default|camtu082880@gmail.com:camtu082880:minhanh|http|42.118.228.99||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="21" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="H15" s="12"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -2081,12 +2286,12 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -2149,12 +2354,12 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
@@ -2243,12 +2448,12 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
@@ -2384,11 +2589,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A5:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2511,29 +2716,29 @@
         <v>5948331720</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+    <row r="8" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
         <v>3</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="10">
         <v>5948331720</v>
       </c>
-      <c r="L8" s="16" t="str">
+      <c r="L8" s="10" t="str">
         <f>CONCATENATE("default|",B8,":",C8,":",D8,"|http|",G8,"|",I8,"|",J8,"|",K8,"|")</f>
         <v>default|phongvuong.info@gmail.com::|http|183.80.65.178||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
@@ -2565,35 +2770,35 @@
         <v>default|phongvuong.info@gmail.com::|http|183.80.65.178||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+    <row r="10" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>5</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="C10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="10">
         <v>5948331720</v>
       </c>
-      <c r="L10" s="16" t="str">
+      <c r="L10" s="10" t="str">
         <f>CONCATENATE("default|",B10,":",C10,":",D10,"|http|",G10,"|",I10,"|",J10,"|",K10,"|")</f>
         <v>default|phongvuong.info@gmail.com:Vuongphong:Nhicolai0789|http|183.80.65.178||5678131708:AAEAHHmegTq0wk6FTETUX5kmFf7MUiUZZiE|5948331720|</v>
       </c>
@@ -2685,26 +2890,26 @@
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
+    <row r="15" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
         <v>9</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="10">
         <v>5948331720</v>
       </c>
     </row>
@@ -2748,11 +2953,11 @@
         <v>31</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
@@ -2861,7 +3066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A5:G60"/>
   <sheetViews>
@@ -3595,7 +3800,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:E60">
+  <autoFilter ref="A5:E60" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="4">
       <filters>
         <filter val="Game"/>
@@ -3603,50 +3808,50 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B9" r:id="rId4"/>
-    <hyperlink ref="B50" r:id="rId5"/>
-    <hyperlink ref="B11" r:id="rId6"/>
-    <hyperlink ref="B10" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B17" r:id="rId13"/>
-    <hyperlink ref="B18" r:id="rId14"/>
-    <hyperlink ref="B19" r:id="rId15"/>
-    <hyperlink ref="B20" r:id="rId16"/>
-    <hyperlink ref="B21" r:id="rId17"/>
-    <hyperlink ref="B22" r:id="rId18"/>
-    <hyperlink ref="B23" r:id="rId19"/>
-    <hyperlink ref="B24" r:id="rId20"/>
-    <hyperlink ref="B25" r:id="rId21"/>
-    <hyperlink ref="B26" r:id="rId22"/>
-    <hyperlink ref="B27" r:id="rId23"/>
-    <hyperlink ref="B28" r:id="rId24"/>
-    <hyperlink ref="B29" r:id="rId25"/>
-    <hyperlink ref="B30" r:id="rId26"/>
-    <hyperlink ref="B31" r:id="rId27"/>
-    <hyperlink ref="B33" r:id="rId28"/>
-    <hyperlink ref="B34" r:id="rId29"/>
-    <hyperlink ref="B35" r:id="rId30"/>
-    <hyperlink ref="B36" r:id="rId31"/>
-    <hyperlink ref="B37" r:id="rId32"/>
-    <hyperlink ref="B38" r:id="rId33"/>
-    <hyperlink ref="B39" r:id="rId34"/>
-    <hyperlink ref="B40" r:id="rId35"/>
-    <hyperlink ref="B41" r:id="rId36"/>
-    <hyperlink ref="B42" r:id="rId37"/>
-    <hyperlink ref="B43" r:id="rId38"/>
-    <hyperlink ref="B44" r:id="rId39"/>
-    <hyperlink ref="B46" r:id="rId40"/>
-    <hyperlink ref="B47" r:id="rId41"/>
-    <hyperlink ref="B49" r:id="rId42"/>
-    <hyperlink ref="B55" r:id="rId43"/>
-    <hyperlink ref="B56" r:id="rId44"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B50" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="B27" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="B28" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="B29" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="B30" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="B31" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="B33" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="B34" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="B35" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="B36" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="B37" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="B38" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="B39" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="B40" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="B41" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="B42" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="B43" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="B44" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="B46" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="B47" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="B49" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="B55" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="B56" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId45"/>
@@ -3654,11 +3859,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:H148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A5:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3677,13 +3882,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -3692,21 +3897,21 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="13" t="s">
         <v>271</v>
       </c>
       <c r="C6" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D6" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -3715,44 +3920,44 @@
         <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="13" t="s">
         <v>272</v>
       </c>
       <c r="C7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
         <v>300</v>
-      </c>
-      <c r="D7" t="s">
-        <v>299</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="13" t="s">
         <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D8" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -3761,21 +3966,21 @@
         <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="13" t="s">
         <v>150</v>
       </c>
       <c r="C9" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D9" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E9" t="s">
         <v>30</v>
@@ -3784,18 +3989,18 @@
         <v>31</v>
       </c>
       <c r="G9" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="13" t="s">
         <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E10" t="s">
         <v>30</v>
@@ -3804,24 +4009,24 @@
         <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H10" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>6</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="13" t="s">
         <v>273</v>
       </c>
       <c r="C11" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -3830,30 +4035,54 @@
         <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>7</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="13" t="s">
         <v>152</v>
+      </c>
+      <c r="C12" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>8</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="13" t="s">
         <v>153</v>
+      </c>
+      <c r="C13" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" t="s">
+        <v>324</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>9</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="13" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3861,527 +4090,974 @@
       <c r="A15">
         <v>10</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="13" t="s">
         <v>155</v>
+      </c>
+      <c r="D15" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>11</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="13" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="C16" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" t="s">
+        <v>327</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A17" s="10">
         <v>12</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>13</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="13" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>14</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="13" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>15</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="13" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>330</v>
+      </c>
+      <c r="D20" t="s">
+        <v>331</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>16</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="13" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="C21" t="s">
+        <v>332</v>
+      </c>
+      <c r="D21" t="s">
+        <v>333</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A22" s="10">
         <v>17</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>18</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="13" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D23" t="s">
+        <v>335</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>19</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="13" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A25">
+      <c r="C24" t="s">
+        <v>336</v>
+      </c>
+      <c r="D24" t="s">
+        <v>337</v>
+      </c>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A25" s="10">
         <v>20</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>21</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>22</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="13" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>338</v>
+      </c>
+      <c r="D27" t="s">
+        <v>339</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>23</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="13" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>340</v>
+      </c>
+      <c r="D28" t="s">
+        <v>341</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>24</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="13" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>342</v>
+      </c>
+      <c r="D29" t="s">
+        <v>343</v>
+      </c>
+      <c r="E29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>25</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="13" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>344</v>
+      </c>
+      <c r="D30" t="s">
+        <v>345</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>26</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="13" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>346</v>
+      </c>
+      <c r="D31" t="s">
+        <v>348</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>27</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="13" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>347</v>
+      </c>
+      <c r="D32" t="s">
+        <v>349</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>28</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="13" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A34">
+      <c r="C33" t="s">
+        <v>350</v>
+      </c>
+      <c r="D33" t="s">
+        <v>351</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A34" s="10">
         <v>29</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>30</v>
-      </c>
-      <c r="B35" s="18" t="s">
+      <c r="B34" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A35" s="10">
+        <v>30</v>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>31</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="13" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>353</v>
+      </c>
+      <c r="D36" t="s">
+        <v>354</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>32</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="13" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A38">
+      <c r="D37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A38" s="10">
         <v>33</v>
       </c>
-      <c r="B38" s="18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B38" s="14" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>34</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="13" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C39" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D39" t="s">
+        <v>359</v>
+      </c>
+      <c r="G39" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>35</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="13" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>360</v>
+      </c>
+      <c r="D40" t="s">
+        <v>362</v>
+      </c>
+      <c r="G40" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>36</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="13" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A42">
+      <c r="C41" t="s">
+        <v>363</v>
+      </c>
+      <c r="D41" t="s">
+        <v>364</v>
+      </c>
+      <c r="G41" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A42" s="10">
         <v>37</v>
       </c>
-      <c r="B42" s="18" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B42" s="14" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>38</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="13" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A44">
+      <c r="C43" t="s">
+        <v>365</v>
+      </c>
+      <c r="D43" t="s">
+        <v>366</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A44" s="10">
         <v>39</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>40</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="13" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>367</v>
+      </c>
+      <c r="D45" t="s">
+        <v>368</v>
+      </c>
+      <c r="E45" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>41</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="13" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C46" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="E46" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>42</v>
       </c>
-      <c r="B47" s="18" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A48">
+      <c r="B47" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C47" t="s">
+        <v>371</v>
+      </c>
+      <c r="D47" t="s">
+        <v>372</v>
+      </c>
+      <c r="E47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A48" s="10">
         <v>43</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="14" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>44</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="13" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>373</v>
+      </c>
+      <c r="D49" t="s">
+        <v>374</v>
+      </c>
+      <c r="E49" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>45</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="13" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A51">
+      <c r="C50" t="s">
+        <v>375</v>
+      </c>
+      <c r="D50" t="s">
+        <v>376</v>
+      </c>
+      <c r="E50" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A51" s="10">
         <v>46</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B51" s="14" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>47</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="13" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C52" t="s">
+        <v>378</v>
+      </c>
+      <c r="D52" t="s">
+        <v>379</v>
+      </c>
+      <c r="E52" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>48</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="13" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C53" t="s">
+        <v>380</v>
+      </c>
+      <c r="D53" t="s">
+        <v>381</v>
+      </c>
+      <c r="E53" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>49</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="13" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C54" t="s">
+        <v>382</v>
+      </c>
+      <c r="D54" t="s">
+        <v>383</v>
+      </c>
+      <c r="E54" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>50</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="13" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A56">
+    <row r="56" spans="1:6" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A56" s="10">
         <v>51</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="14" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>52</v>
       </c>
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="13" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C57" t="s">
+        <v>385</v>
+      </c>
+      <c r="D57" t="s">
+        <v>386</v>
+      </c>
+      <c r="E57" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>53</v>
       </c>
-      <c r="B58" s="18" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B58" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C58" t="s">
+        <v>389</v>
+      </c>
+      <c r="D58" t="s">
+        <v>387</v>
+      </c>
+      <c r="E58" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>54</v>
       </c>
-      <c r="B59" s="18" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B59" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C59" t="s">
+        <v>390</v>
+      </c>
+      <c r="D59" t="s">
+        <v>391</v>
+      </c>
+      <c r="E59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>55</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B60" s="13" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>56</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="13" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A62">
+      <c r="C61" t="s">
+        <v>392</v>
+      </c>
+      <c r="D61" t="s">
+        <v>393</v>
+      </c>
+      <c r="E61" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A62" s="10">
         <v>57</v>
       </c>
-      <c r="B62" s="18" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A63">
+      <c r="B62" s="14" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A63" s="10">
         <v>58</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B63" s="14" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>59</v>
       </c>
-      <c r="B64" s="18" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B64" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C64" t="s">
+        <v>396</v>
+      </c>
+      <c r="D64" t="s">
+        <v>397</v>
+      </c>
+      <c r="E64" t="s">
+        <v>30</v>
+      </c>
+      <c r="F64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>60</v>
       </c>
-      <c r="B65" s="18" t="s">
+      <c r="B65" s="13" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" t="s">
+        <v>398</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>61</v>
       </c>
-      <c r="B66" s="18" t="s">
+      <c r="B66" s="13" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C66" t="s">
+        <v>399</v>
+      </c>
+      <c r="D66" t="s">
+        <v>400</v>
+      </c>
+      <c r="E66" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>62</v>
       </c>
-      <c r="B67" s="18" t="s">
+      <c r="B67" s="13" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C67" t="s">
+        <v>401</v>
+      </c>
+      <c r="D67" t="s">
+        <v>402</v>
+      </c>
+      <c r="E67" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>63</v>
       </c>
-      <c r="B68" s="18" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B68" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C68" t="s">
+        <v>403</v>
+      </c>
+      <c r="D68" t="s">
+        <v>404</v>
+      </c>
+      <c r="E68" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>64</v>
       </c>
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="13" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C69" t="s">
+        <v>405</v>
+      </c>
+      <c r="D69" t="s">
+        <v>406</v>
+      </c>
+      <c r="E69" t="s">
+        <v>30</v>
+      </c>
+      <c r="F69" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>65</v>
       </c>
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="13" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C70" t="s">
+        <v>407</v>
+      </c>
+      <c r="D70" t="s">
+        <v>408</v>
+      </c>
+      <c r="E70" t="s">
+        <v>30</v>
+      </c>
+      <c r="F70" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>66</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="13" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="C71" t="s">
+        <v>409</v>
+      </c>
+      <c r="D71" t="s">
+        <v>410</v>
+      </c>
+      <c r="E71" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>67</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="13" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>68</v>
       </c>
-      <c r="B73" s="18" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="B73" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>69</v>
       </c>
-      <c r="B74" s="18" t="s">
+      <c r="B74" s="13" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>70</v>
       </c>
-      <c r="B75" s="18" t="s">
+      <c r="B75" s="13" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>71</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>72</v>
       </c>
-      <c r="B77" s="18" t="s">
+      <c r="B77" s="13" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>73</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="13" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>74</v>
       </c>
-      <c r="B79" s="18" t="s">
+      <c r="B79" s="13" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>75</v>
       </c>
-      <c r="B80" s="18" t="s">
+      <c r="B80" s="13" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4389,7 +5065,7 @@
       <c r="A81">
         <v>76</v>
       </c>
-      <c r="B81" s="18" t="s">
+      <c r="B81" s="13" t="s">
         <v>208</v>
       </c>
     </row>
@@ -4397,7 +5073,7 @@
       <c r="A82">
         <v>77</v>
       </c>
-      <c r="B82" s="18" t="s">
+      <c r="B82" s="13" t="s">
         <v>209</v>
       </c>
     </row>
@@ -4405,7 +5081,7 @@
       <c r="A83">
         <v>78</v>
       </c>
-      <c r="B83" s="18" t="s">
+      <c r="B83" s="13" t="s">
         <v>210</v>
       </c>
     </row>
@@ -4413,7 +5089,7 @@
       <c r="A84">
         <v>79</v>
       </c>
-      <c r="B84" s="18" t="s">
+      <c r="B84" s="13" t="s">
         <v>211</v>
       </c>
     </row>
@@ -4421,7 +5097,7 @@
       <c r="A85">
         <v>80</v>
       </c>
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="13" t="s">
         <v>212</v>
       </c>
     </row>
@@ -4429,15 +5105,15 @@
       <c r="A86">
         <v>81</v>
       </c>
-      <c r="B86" s="18" t="s">
-        <v>287</v>
+      <c r="B86" s="13" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>82</v>
       </c>
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="13" t="s">
         <v>213</v>
       </c>
     </row>
@@ -4445,7 +5121,7 @@
       <c r="A88">
         <v>83</v>
       </c>
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="13" t="s">
         <v>214</v>
       </c>
     </row>
@@ -4453,7 +5129,7 @@
       <c r="A89">
         <v>84</v>
       </c>
-      <c r="B89" s="18" t="s">
+      <c r="B89" s="13" t="s">
         <v>215</v>
       </c>
     </row>
@@ -4461,15 +5137,15 @@
       <c r="A90">
         <v>85</v>
       </c>
-      <c r="B90" s="18" t="s">
-        <v>288</v>
+      <c r="B90" s="13" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>86</v>
       </c>
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="13" t="s">
         <v>216</v>
       </c>
     </row>
@@ -4477,7 +5153,7 @@
       <c r="A92">
         <v>87</v>
       </c>
-      <c r="B92" s="18" t="s">
+      <c r="B92" s="13" t="s">
         <v>217</v>
       </c>
     </row>
@@ -4485,7 +5161,7 @@
       <c r="A93">
         <v>88</v>
       </c>
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="13" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4493,7 +5169,7 @@
       <c r="A94">
         <v>89</v>
       </c>
-      <c r="B94" s="18" t="s">
+      <c r="B94" s="13" t="s">
         <v>219</v>
       </c>
     </row>
@@ -4501,7 +5177,7 @@
       <c r="A95">
         <v>90</v>
       </c>
-      <c r="B95" s="18" t="s">
+      <c r="B95" s="13" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4509,7 +5185,7 @@
       <c r="A96">
         <v>91</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="13" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4517,7 +5193,7 @@
       <c r="A97">
         <v>92</v>
       </c>
-      <c r="B97" s="18" t="s">
+      <c r="B97" s="13" t="s">
         <v>222</v>
       </c>
     </row>
@@ -4525,7 +5201,7 @@
       <c r="A98">
         <v>93</v>
       </c>
-      <c r="B98" s="18" t="s">
+      <c r="B98" s="13" t="s">
         <v>223</v>
       </c>
     </row>
@@ -4533,7 +5209,7 @@
       <c r="A99">
         <v>94</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="13" t="s">
         <v>224</v>
       </c>
     </row>
@@ -4541,7 +5217,7 @@
       <c r="A100">
         <v>95</v>
       </c>
-      <c r="B100" s="18" t="s">
+      <c r="B100" s="13" t="s">
         <v>225</v>
       </c>
     </row>
@@ -4549,7 +5225,7 @@
       <c r="A101">
         <v>96</v>
       </c>
-      <c r="B101" s="18" t="s">
+      <c r="B101" s="13" t="s">
         <v>226</v>
       </c>
     </row>
@@ -4557,7 +5233,7 @@
       <c r="A102">
         <v>97</v>
       </c>
-      <c r="B102" s="18" t="s">
+      <c r="B102" s="13" t="s">
         <v>227</v>
       </c>
     </row>
@@ -4565,7 +5241,7 @@
       <c r="A103">
         <v>98</v>
       </c>
-      <c r="B103" s="18" t="s">
+      <c r="B103" s="13" t="s">
         <v>228</v>
       </c>
     </row>
@@ -4573,7 +5249,7 @@
       <c r="A104">
         <v>99</v>
       </c>
-      <c r="B104" s="18" t="s">
+      <c r="B104" s="13" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4581,7 +5257,7 @@
       <c r="A105">
         <v>100</v>
       </c>
-      <c r="B105" s="18" t="s">
+      <c r="B105" s="13" t="s">
         <v>230</v>
       </c>
     </row>
@@ -4589,7 +5265,7 @@
       <c r="A106">
         <v>101</v>
       </c>
-      <c r="B106" s="18" t="s">
+      <c r="B106" s="13" t="s">
         <v>231</v>
       </c>
     </row>
@@ -4597,7 +5273,7 @@
       <c r="A107">
         <v>102</v>
       </c>
-      <c r="B107" s="18" t="s">
+      <c r="B107" s="13" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4605,7 +5281,7 @@
       <c r="A108">
         <v>103</v>
       </c>
-      <c r="B108" s="18" t="s">
+      <c r="B108" s="13" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4613,7 +5289,7 @@
       <c r="A109">
         <v>104</v>
       </c>
-      <c r="B109" s="18" t="s">
+      <c r="B109" s="13" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4621,7 +5297,7 @@
       <c r="A110">
         <v>105</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="13" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4629,7 +5305,7 @@
       <c r="A111">
         <v>106</v>
       </c>
-      <c r="B111" s="18" t="s">
+      <c r="B111" s="13" t="s">
         <v>236</v>
       </c>
     </row>
@@ -4637,7 +5313,7 @@
       <c r="A112">
         <v>107</v>
       </c>
-      <c r="B112" s="18" t="s">
+      <c r="B112" s="13" t="s">
         <v>237</v>
       </c>
     </row>
@@ -4645,7 +5321,7 @@
       <c r="A113">
         <v>108</v>
       </c>
-      <c r="B113" s="18" t="s">
+      <c r="B113" s="13" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4653,7 +5329,7 @@
       <c r="A114">
         <v>109</v>
       </c>
-      <c r="B114" s="18" t="s">
+      <c r="B114" s="13" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4661,7 +5337,7 @@
       <c r="A115">
         <v>110</v>
       </c>
-      <c r="B115" s="18" t="s">
+      <c r="B115" s="13" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4669,7 +5345,7 @@
       <c r="A116">
         <v>111</v>
       </c>
-      <c r="B116" s="18" t="s">
+      <c r="B116" s="13" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4677,7 +5353,7 @@
       <c r="A117">
         <v>112</v>
       </c>
-      <c r="B117" s="18" t="s">
+      <c r="B117" s="13" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4685,7 +5361,7 @@
       <c r="A118">
         <v>113</v>
       </c>
-      <c r="B118" s="18" t="s">
+      <c r="B118" s="13" t="s">
         <v>243</v>
       </c>
     </row>
@@ -4693,15 +5369,15 @@
       <c r="A119">
         <v>114</v>
       </c>
-      <c r="B119" s="18" t="s">
-        <v>289</v>
+      <c r="B119" s="13" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>115</v>
       </c>
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="13" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4709,7 +5385,7 @@
       <c r="A121">
         <v>116</v>
       </c>
-      <c r="B121" s="18" t="s">
+      <c r="B121" s="13" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4717,7 +5393,7 @@
       <c r="A122">
         <v>117</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="13" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4725,7 +5401,7 @@
       <c r="A123">
         <v>118</v>
       </c>
-      <c r="B123" s="18" t="s">
+      <c r="B123" s="13" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4733,7 +5409,7 @@
       <c r="A124">
         <v>119</v>
       </c>
-      <c r="B124" s="18" t="s">
+      <c r="B124" s="13" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4741,7 +5417,7 @@
       <c r="A125">
         <v>120</v>
       </c>
-      <c r="B125" s="18" t="s">
+      <c r="B125" s="13" t="s">
         <v>249</v>
       </c>
     </row>
@@ -4749,7 +5425,7 @@
       <c r="A126">
         <v>121</v>
       </c>
-      <c r="B126" s="18" t="s">
+      <c r="B126" s="13" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4757,7 +5433,7 @@
       <c r="A127">
         <v>122</v>
       </c>
-      <c r="B127" s="18" t="s">
+      <c r="B127" s="13" t="s">
         <v>251</v>
       </c>
     </row>
@@ -4765,7 +5441,7 @@
       <c r="A128">
         <v>123</v>
       </c>
-      <c r="B128" s="18" t="s">
+      <c r="B128" s="13" t="s">
         <v>252</v>
       </c>
     </row>
@@ -4773,15 +5449,15 @@
       <c r="A129">
         <v>124</v>
       </c>
-      <c r="B129" s="18" t="s">
-        <v>290</v>
+      <c r="B129" s="13" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>125</v>
       </c>
-      <c r="B130" s="18" t="s">
+      <c r="B130" s="13" t="s">
         <v>253</v>
       </c>
     </row>
@@ -4789,7 +5465,7 @@
       <c r="A131">
         <v>126</v>
       </c>
-      <c r="B131" s="18" t="s">
+      <c r="B131" s="13" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4797,7 +5473,7 @@
       <c r="A132">
         <v>127</v>
       </c>
-      <c r="B132" s="18" t="s">
+      <c r="B132" s="13" t="s">
         <v>255</v>
       </c>
     </row>
@@ -4805,7 +5481,7 @@
       <c r="A133">
         <v>128</v>
       </c>
-      <c r="B133" s="18" t="s">
+      <c r="B133" s="13" t="s">
         <v>256</v>
       </c>
     </row>
@@ -4813,7 +5489,7 @@
       <c r="A134">
         <v>129</v>
       </c>
-      <c r="B134" s="18" t="s">
+      <c r="B134" s="13" t="s">
         <v>257</v>
       </c>
     </row>
@@ -4821,7 +5497,7 @@
       <c r="A135">
         <v>130</v>
       </c>
-      <c r="B135" s="18" t="s">
+      <c r="B135" s="13" t="s">
         <v>258</v>
       </c>
     </row>
@@ -4829,7 +5505,7 @@
       <c r="A136">
         <v>131</v>
       </c>
-      <c r="B136" s="18" t="s">
+      <c r="B136" s="13" t="s">
         <v>259</v>
       </c>
     </row>
@@ -4837,7 +5513,7 @@
       <c r="A137">
         <v>132</v>
       </c>
-      <c r="B137" s="18" t="s">
+      <c r="B137" s="13" t="s">
         <v>260</v>
       </c>
     </row>
@@ -4845,7 +5521,7 @@
       <c r="A138">
         <v>133</v>
       </c>
-      <c r="B138" s="18" t="s">
+      <c r="B138" s="13" t="s">
         <v>261</v>
       </c>
     </row>
@@ -4853,7 +5529,7 @@
       <c r="A139">
         <v>134</v>
       </c>
-      <c r="B139" s="18" t="s">
+      <c r="B139" s="13" t="s">
         <v>262</v>
       </c>
     </row>
@@ -4861,23 +5537,23 @@
       <c r="A140">
         <v>135</v>
       </c>
-      <c r="B140" s="18" t="s">
+      <c r="B140" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="H140" s="20"/>
+      <c r="H140" s="15"/>
     </row>
     <row r="141" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>136</v>
       </c>
-      <c r="B141" s="18" t="s">
+      <c r="B141" s="13" t="s">
         <v>264</v>
       </c>
       <c r="C141" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D141" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E141" t="s">
         <v>30</v>
@@ -4886,22 +5562,22 @@
         <v>31</v>
       </c>
       <c r="G141" t="s">
-        <v>298</v>
-      </c>
-      <c r="H141" s="20"/>
+        <v>293</v>
+      </c>
+      <c r="H141" s="15"/>
     </row>
     <row r="142" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>137</v>
       </c>
-      <c r="B142" s="18" t="s">
+      <c r="B142" s="13" t="s">
         <v>265</v>
       </c>
       <c r="C142" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D142" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E142" t="s">
         <v>30</v>
@@ -4910,24 +5586,24 @@
         <v>31</v>
       </c>
       <c r="G142" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H142" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>138</v>
       </c>
-      <c r="B143" s="18" t="s">
+      <c r="B143" s="13" t="s">
         <v>266</v>
       </c>
       <c r="C143" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D143" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E143" t="s">
         <v>29</v>
@@ -4936,21 +5612,21 @@
         <v>31</v>
       </c>
       <c r="G143" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>139</v>
       </c>
-      <c r="B144" s="18" t="s">
+      <c r="B144" s="13" t="s">
         <v>267</v>
       </c>
       <c r="C144" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D144" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E144" t="s">
         <v>29</v>
@@ -4959,21 +5635,21 @@
         <v>31</v>
       </c>
       <c r="G144" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>140</v>
       </c>
-      <c r="B145" s="18" t="s">
+      <c r="B145" s="13" t="s">
         <v>268</v>
       </c>
       <c r="C145" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D145" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E145" t="s">
         <v>30</v>
@@ -4982,17 +5658,17 @@
         <v>31</v>
       </c>
       <c r="G145" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H145" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.35">
-      <c r="A146" s="16">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A146" s="10">
         <v>141</v>
       </c>
-      <c r="B146" s="19" t="s">
+      <c r="B146" s="14" t="s">
         <v>269</v>
       </c>
     </row>
@@ -5000,14 +5676,14 @@
       <c r="A147">
         <v>142</v>
       </c>
-      <c r="B147" s="18" t="s">
+      <c r="B147" s="13" t="s">
         <v>270</v>
       </c>
       <c r="C147" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D147" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E147" t="s">
         <v>30</v>
@@ -5016,21 +5692,21 @@
         <v>31</v>
       </c>
       <c r="G147" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>143</v>
       </c>
-      <c r="B148" s="18" t="s">
-        <v>291</v>
+      <c r="B148" s="13" t="s">
+        <v>286</v>
       </c>
       <c r="C148" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D148" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E148" t="s">
         <v>30</v>
@@ -5039,11 +5715,44 @@
         <v>31</v>
       </c>
       <c r="G148" t="s">
-        <v>298</v>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C149" t="s">
+        <v>384</v>
+      </c>
+      <c r="E149" t="s">
+        <v>30</v>
+      </c>
+      <c r="F149" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C150" t="s">
+        <v>388</v>
+      </c>
+      <c r="E150" t="s">
+        <v>30</v>
+      </c>
+      <c r="F150" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C151" t="s">
+        <v>394</v>
+      </c>
+      <c r="E151" t="s">
+        <v>30</v>
+      </c>
+      <c r="F151" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>